<commit_message>
Data cleaning for analysis in R
</commit_message>
<xml_diff>
--- a/data files/artificial-nectar_yeast_gr_9-7-21.xlsx
+++ b/data files/artificial-nectar_yeast_gr_9-7-21.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Experiments\Elizabeth Moore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melmo\Documents\Bee-Yeast experiments\artificial-nectar_trials\data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86FB12C-E0AF-4D5D-A0A2-7FE5A8DA7EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="9435" windowHeight="6915"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="plate key" sheetId="2" r:id="rId2"/>
+    <sheet name="well key" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="MethodPointer1">-462737472</definedName>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="286">
   <si>
     <t>Software Version</t>
   </si>
@@ -513,12 +516,381 @@
   <si>
     <t>Lagtime [600]</t>
   </si>
+  <si>
+    <t>well_id</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>strain_trt_id</t>
+  </si>
+  <si>
+    <t>430_hiye</t>
+  </si>
+  <si>
+    <t>432_hiye</t>
+  </si>
+  <si>
+    <t>466_hiye</t>
+  </si>
+  <si>
+    <t>470_hiye</t>
+  </si>
+  <si>
+    <t>476_hiye</t>
+  </si>
+  <si>
+    <t>477_hiye</t>
+  </si>
+  <si>
+    <t>478_hiye</t>
+  </si>
+  <si>
+    <t>480_hiye</t>
+  </si>
+  <si>
+    <t>485_hiye</t>
+  </si>
+  <si>
+    <t>583_hiye</t>
+  </si>
+  <si>
+    <t>430_lowye</t>
+  </si>
+  <si>
+    <t>432_lowye</t>
+  </si>
+  <si>
+    <t>466_lowye</t>
+  </si>
+  <si>
+    <t>470_lowye</t>
+  </si>
+  <si>
+    <t>476_lowye</t>
+  </si>
+  <si>
+    <t>477_lowye</t>
+  </si>
+  <si>
+    <t>478_lowye</t>
+  </si>
+  <si>
+    <t>480_lowye</t>
+  </si>
+  <si>
+    <t>485_lowye</t>
+  </si>
+  <si>
+    <t>583_lowye</t>
+  </si>
+  <si>
+    <t>strain_trt_rep_id</t>
+  </si>
+  <si>
+    <t>plate_id</t>
+  </si>
+  <si>
+    <t>blank_1</t>
+  </si>
+  <si>
+    <t>blank_2</t>
+  </si>
+  <si>
+    <t>blank_3</t>
+  </si>
+  <si>
+    <t>blank_4</t>
+  </si>
+  <si>
+    <t>blank_5</t>
+  </si>
+  <si>
+    <t>blank_6</t>
+  </si>
+  <si>
+    <t>blank_7</t>
+  </si>
+  <si>
+    <t>blank_8</t>
+  </si>
+  <si>
+    <t>blank_9</t>
+  </si>
+  <si>
+    <t>blank_10</t>
+  </si>
+  <si>
+    <t>blank_11</t>
+  </si>
+  <si>
+    <t>blank_12</t>
+  </si>
+  <si>
+    <t>blank_13</t>
+  </si>
+  <si>
+    <t>blank_14</t>
+  </si>
+  <si>
+    <t>blank_15</t>
+  </si>
+  <si>
+    <t>blank_16</t>
+  </si>
+  <si>
+    <t>blank_17</t>
+  </si>
+  <si>
+    <t>blank_18</t>
+  </si>
+  <si>
+    <t>blank_19</t>
+  </si>
+  <si>
+    <t>blank_20</t>
+  </si>
+  <si>
+    <t>blank_21</t>
+  </si>
+  <si>
+    <t>blank_22</t>
+  </si>
+  <si>
+    <t>blank_23</t>
+  </si>
+  <si>
+    <t>blank_24</t>
+  </si>
+  <si>
+    <t>blank_25</t>
+  </si>
+  <si>
+    <t>blank_26</t>
+  </si>
+  <si>
+    <t>blank_27</t>
+  </si>
+  <si>
+    <t>blank_28</t>
+  </si>
+  <si>
+    <t>blank_29</t>
+  </si>
+  <si>
+    <t>blank_30</t>
+  </si>
+  <si>
+    <t>blank_31</t>
+  </si>
+  <si>
+    <t>blank_32</t>
+  </si>
+  <si>
+    <t>blank_33</t>
+  </si>
+  <si>
+    <t>blank_34</t>
+  </si>
+  <si>
+    <t>blank_35</t>
+  </si>
+  <si>
+    <t>blank_36</t>
+  </si>
+  <si>
+    <t>blank_hiye</t>
+  </si>
+  <si>
+    <t>blank_lowye</t>
+  </si>
+  <si>
+    <t>430_hiye_1</t>
+  </si>
+  <si>
+    <t>430_hiye_2</t>
+  </si>
+  <si>
+    <t>430_hiye_3</t>
+  </si>
+  <si>
+    <t>432_hiye_2</t>
+  </si>
+  <si>
+    <t>432_hiye_1</t>
+  </si>
+  <si>
+    <t>432_hiye_3</t>
+  </si>
+  <si>
+    <t>466_hiye_1</t>
+  </si>
+  <si>
+    <t>466_hiye_2</t>
+  </si>
+  <si>
+    <t>466_hiye_3</t>
+  </si>
+  <si>
+    <t>470_hiye_1</t>
+  </si>
+  <si>
+    <t>470_hiye_2</t>
+  </si>
+  <si>
+    <t>470_hiye_3</t>
+  </si>
+  <si>
+    <t>476_hiye_1</t>
+  </si>
+  <si>
+    <t>476_hiye_2</t>
+  </si>
+  <si>
+    <t>476_hiye_3</t>
+  </si>
+  <si>
+    <t>477_hiye_1</t>
+  </si>
+  <si>
+    <t>477_hiye_2</t>
+  </si>
+  <si>
+    <t>477_hiye_3</t>
+  </si>
+  <si>
+    <t>478_hiye_1</t>
+  </si>
+  <si>
+    <t>478_hiye_2</t>
+  </si>
+  <si>
+    <t>478_hiye_3</t>
+  </si>
+  <si>
+    <t>480_hiye_1</t>
+  </si>
+  <si>
+    <t>480_hiye_2</t>
+  </si>
+  <si>
+    <t>480_hiye_3</t>
+  </si>
+  <si>
+    <t>485_hiye_1</t>
+  </si>
+  <si>
+    <t>485_hiye_2</t>
+  </si>
+  <si>
+    <t>485_hiye_3</t>
+  </si>
+  <si>
+    <t>583_hiye_1</t>
+  </si>
+  <si>
+    <t>583_hiye_2</t>
+  </si>
+  <si>
+    <t>583_hiye_3</t>
+  </si>
+  <si>
+    <t>430_lowye_1</t>
+  </si>
+  <si>
+    <t>430_lowye_2</t>
+  </si>
+  <si>
+    <t>430_lowye_3</t>
+  </si>
+  <si>
+    <t>432_lowye_1</t>
+  </si>
+  <si>
+    <t>432_lowye_2</t>
+  </si>
+  <si>
+    <t>432_lowye_3</t>
+  </si>
+  <si>
+    <t>466_lowye_1</t>
+  </si>
+  <si>
+    <t>466_lowye_2</t>
+  </si>
+  <si>
+    <t>466_lowye_3</t>
+  </si>
+  <si>
+    <t>470_lowye_1</t>
+  </si>
+  <si>
+    <t>470_lowye_2</t>
+  </si>
+  <si>
+    <t>470_lowye_3</t>
+  </si>
+  <si>
+    <t>476_lowye_1</t>
+  </si>
+  <si>
+    <t>476_lowye_2</t>
+  </si>
+  <si>
+    <t>476_lowye_3</t>
+  </si>
+  <si>
+    <t>477_lowye_1</t>
+  </si>
+  <si>
+    <t>477_lowye_2</t>
+  </si>
+  <si>
+    <t>477_lowye_3</t>
+  </si>
+  <si>
+    <t>478_lowye_1</t>
+  </si>
+  <si>
+    <t>478_lowye_2</t>
+  </si>
+  <si>
+    <t>478_lowye_3</t>
+  </si>
+  <si>
+    <t>480_lowye_1</t>
+  </si>
+  <si>
+    <t>480_lowye_2</t>
+  </si>
+  <si>
+    <t>480_lowye_3</t>
+  </si>
+  <si>
+    <t>485_lowye_1</t>
+  </si>
+  <si>
+    <t>485_lowye_2</t>
+  </si>
+  <si>
+    <t>485_lowye_3</t>
+  </si>
+  <si>
+    <t>583_lowye_1</t>
+  </si>
+  <si>
+    <t>583_lowye_2</t>
+  </si>
+  <si>
+    <t>583_lowye_3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -549,6 +921,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -570,7 +961,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -630,11 +1021,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -695,6 +1131,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,20 +1424,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:CU267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B235" sqref="B235"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -995,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1003,7 +1453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1011,7 +1461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1019,7 +1469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1027,7 +1477,7 @@
         <v>44446</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1035,7 +1485,7 @@
         <v>0.51784722222222224</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1043,7 +1493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1501,7 @@
         <v>21012810</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1059,13 +1509,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1073,7 +1523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1081,7 +1531,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1089,12 +1539,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1102,33 +1552,33 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="6">
         <v>1</v>
@@ -1167,7 +1617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1211,7 +1661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>33</v>
       </c>
@@ -1255,7 +1705,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>44</v>
       </c>
@@ -1299,7 +1749,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>45</v>
       </c>
@@ -1343,7 +1793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>46</v>
       </c>
@@ -1387,7 +1837,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>57</v>
       </c>
@@ -1431,7 +1881,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>58</v>
       </c>
@@ -1475,7 +1925,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>59</v>
       </c>
@@ -1519,13 +1969,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:99" ht="13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>600</v>
       </c>
       <c r="B36" s="4"/>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>9</v>
       </c>
@@ -1821,7 +2271,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B39" s="9">
         <v>9.9074074074074082E-3</v>
       </c>
@@ -2117,7 +2567,7 @@
         <v>0.71799999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B40" s="9">
         <v>2.0324074074074074E-2</v>
       </c>
@@ -2413,7 +2863,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B41" s="9">
         <v>3.0740740740740739E-2</v>
       </c>
@@ -2709,7 +3159,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B42" s="9">
         <v>4.1157407407407406E-2</v>
       </c>
@@ -3005,7 +3455,7 @@
         <v>0.71399999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B43" s="9">
         <v>5.1574074074074078E-2</v>
       </c>
@@ -3301,7 +3751,7 @@
         <v>0.71399999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B44" s="9">
         <v>6.1990740740740735E-2</v>
       </c>
@@ -3597,7 +4047,7 @@
         <v>0.71299999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B45" s="9">
         <v>7.2407407407407406E-2</v>
       </c>
@@ -3893,7 +4343,7 @@
         <v>0.71299999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B46" s="9">
         <v>8.2824074074074064E-2</v>
       </c>
@@ -4189,7 +4639,7 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B47" s="9">
         <v>9.3240740740740735E-2</v>
       </c>
@@ -4485,7 +4935,7 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B48" s="9">
         <v>0.10365740740740741</v>
       </c>
@@ -4781,7 +5231,7 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="49" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B49" s="9">
         <v>0.11407407407407406</v>
       </c>
@@ -5077,7 +5527,7 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="50" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B50" s="9">
         <v>0.12449074074074074</v>
       </c>
@@ -5373,7 +5823,7 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="51" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B51" s="9">
         <v>0.13490740740740739</v>
       </c>
@@ -5669,7 +6119,7 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="52" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B52" s="9">
         <v>0.14532407407407408</v>
       </c>
@@ -5965,7 +6415,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="53" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B53" s="9">
         <v>0.15574074074074074</v>
       </c>
@@ -6261,7 +6711,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="54" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B54" s="9">
         <v>0.16615740740740739</v>
       </c>
@@ -6557,7 +7007,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="55" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B55" s="9">
         <v>0.17657407407407408</v>
       </c>
@@ -6853,7 +7303,7 @@
         <v>0.70899999999999996</v>
       </c>
     </row>
-    <row r="56" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B56" s="9">
         <v>0.18699074074074074</v>
       </c>
@@ -7149,7 +7599,7 @@
         <v>0.70899999999999996</v>
       </c>
     </row>
-    <row r="57" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B57" s="9">
         <v>0.19740740740740739</v>
       </c>
@@ -7445,7 +7895,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="58" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B58" s="9">
         <v>0.20782407407407408</v>
       </c>
@@ -7741,7 +8191,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="59" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B59" s="9">
         <v>0.21824074074074074</v>
       </c>
@@ -8037,7 +8487,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="60" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B60" s="9">
         <v>0.22865740740740739</v>
       </c>
@@ -8333,7 +8783,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="61" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B61" s="9">
         <v>0.23907407407407408</v>
       </c>
@@ -8629,7 +9079,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="62" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B62" s="9">
         <v>0.24949074074074074</v>
       </c>
@@ -8925,7 +9375,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="63" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B63" s="9">
         <v>0.25990740740740742</v>
       </c>
@@ -9221,7 +9671,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="64" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B64" s="9">
         <v>0.27032407407407405</v>
       </c>
@@ -9517,7 +9967,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="65" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B65" s="9">
         <v>0.28074074074074074</v>
       </c>
@@ -9813,7 +10263,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="66" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B66" s="9">
         <v>0.29115740740740742</v>
       </c>
@@ -10109,7 +10559,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="67" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B67" s="9">
         <v>0.30157407407407405</v>
       </c>
@@ -10405,7 +10855,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="68" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B68" s="9">
         <v>0.31199074074074074</v>
       </c>
@@ -10701,7 +11151,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="69" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B69" s="9">
         <v>0.32240740740740742</v>
       </c>
@@ -10997,7 +11447,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="70" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B70" s="9">
         <v>0.33282407407407405</v>
       </c>
@@ -11293,7 +11743,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="71" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B71" s="9">
         <v>0.34324074074074074</v>
       </c>
@@ -11589,7 +12039,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="72" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B72" s="9">
         <v>0.35365740740740742</v>
       </c>
@@ -11885,7 +12335,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="73" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B73" s="9">
         <v>0.36407407407407405</v>
       </c>
@@ -12181,7 +12631,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="74" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B74" s="9">
         <v>0.37449074074074074</v>
       </c>
@@ -12477,7 +12927,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="75" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B75" s="9">
         <v>0.38490740740740742</v>
       </c>
@@ -12773,7 +13223,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="76" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B76" s="9">
         <v>0.39532407407407405</v>
       </c>
@@ -13069,7 +13519,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="77" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B77" s="9">
         <v>0.40574074074074074</v>
       </c>
@@ -13365,7 +13815,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="78" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B78" s="9">
         <v>0.41615740740740742</v>
       </c>
@@ -13661,7 +14111,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="79" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B79" s="9">
         <v>0.42657407407407405</v>
       </c>
@@ -13957,7 +14407,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="80" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B80" s="9">
         <v>0.43699074074074074</v>
       </c>
@@ -14253,7 +14703,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="81" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B81" s="9">
         <v>0.44740740740740742</v>
       </c>
@@ -14549,7 +14999,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="82" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B82" s="9">
         <v>0.45782407407407405</v>
       </c>
@@ -14845,7 +15295,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="83" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B83" s="9">
         <v>0.46824074074074074</v>
       </c>
@@ -15141,7 +15591,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="84" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B84" s="9">
         <v>0.47865740740740742</v>
       </c>
@@ -15437,7 +15887,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="85" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B85" s="9">
         <v>0.48907407407407405</v>
       </c>
@@ -15733,7 +16183,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="86" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B86" s="9">
         <v>0.49949074074074074</v>
       </c>
@@ -16029,7 +16479,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="87" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B87" s="9">
         <v>0.50990740740740736</v>
       </c>
@@ -16325,7 +16775,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="88" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B88" s="9">
         <v>0.52032407407407411</v>
       </c>
@@ -16621,7 +17071,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="89" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B89" s="9">
         <v>0.53074074074074074</v>
       </c>
@@ -16917,7 +17367,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="90" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B90" s="9">
         <v>0.54115740740740736</v>
       </c>
@@ -17213,7 +17663,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="91" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B91" s="9">
         <v>0.55157407407407411</v>
       </c>
@@ -17509,7 +17959,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="92" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B92" s="9">
         <v>0.56199074074074074</v>
       </c>
@@ -17805,7 +18255,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="93" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B93" s="9">
         <v>0.57240740740740736</v>
       </c>
@@ -18101,7 +18551,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="94" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B94" s="9">
         <v>0.58282407407407411</v>
       </c>
@@ -18397,7 +18847,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="95" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B95" s="9">
         <v>0.59324074074074074</v>
       </c>
@@ -18693,7 +19143,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="96" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B96" s="9">
         <v>0.60365740740740736</v>
       </c>
@@ -18989,7 +19439,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="97" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B97" s="9">
         <v>0.61407407407407411</v>
       </c>
@@ -19285,7 +19735,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="98" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B98" s="9">
         <v>0.62449074074074074</v>
       </c>
@@ -19581,7 +20031,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="99" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B99" s="9">
         <v>0.63490740740740736</v>
       </c>
@@ -19877,7 +20327,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="100" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B100" s="9">
         <v>0.64532407407407411</v>
       </c>
@@ -20173,7 +20623,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="101" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B101" s="9">
         <v>0.65574074074074074</v>
       </c>
@@ -20469,7 +20919,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="102" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B102" s="9">
         <v>0.66615740740740736</v>
       </c>
@@ -20765,7 +21215,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="103" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B103" s="9">
         <v>0.67657407407407411</v>
       </c>
@@ -21061,7 +21511,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="104" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B104" s="9">
         <v>0.68699074074074085</v>
       </c>
@@ -21357,7 +21807,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="105" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B105" s="9">
         <v>0.69740740740740748</v>
       </c>
@@ -21653,7 +22103,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="106" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B106" s="9">
         <v>0.70782407407407411</v>
       </c>
@@ -21949,7 +22399,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="107" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B107" s="9">
         <v>0.71824074074074085</v>
       </c>
@@ -22245,7 +22695,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="108" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B108" s="9">
         <v>0.72865740740740748</v>
       </c>
@@ -22541,7 +22991,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="109" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B109" s="9">
         <v>0.73907407407407411</v>
       </c>
@@ -22837,7 +23287,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="110" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B110" s="9">
         <v>0.74949074074074085</v>
       </c>
@@ -23133,7 +23583,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="111" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B111" s="9">
         <v>0.75990740740740748</v>
       </c>
@@ -23429,7 +23879,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="112" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B112" s="9">
         <v>0.77032407407407411</v>
       </c>
@@ -23725,7 +24175,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="113" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B113" s="9">
         <v>0.78074074074074085</v>
       </c>
@@ -24021,7 +24471,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="114" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B114" s="9">
         <v>0.79115740740740748</v>
       </c>
@@ -24317,7 +24767,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="115" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B115" s="9">
         <v>0.80157407407407411</v>
       </c>
@@ -24613,7 +25063,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="116" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B116" s="9">
         <v>0.81199074074074085</v>
       </c>
@@ -24909,7 +25359,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="117" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B117" s="9">
         <v>0.82240740740740748</v>
       </c>
@@ -25205,7 +25655,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="118" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B118" s="9">
         <v>0.83282407407407411</v>
       </c>
@@ -25501,7 +25951,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="119" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B119" s="9">
         <v>0.84324074074074085</v>
       </c>
@@ -25797,7 +26247,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="120" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B120" s="9">
         <v>0.85365740740740748</v>
       </c>
@@ -26093,7 +26543,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="121" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B121" s="9">
         <v>0.86407407407407411</v>
       </c>
@@ -26389,7 +26839,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="122" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B122" s="9">
         <v>0.87449074074074085</v>
       </c>
@@ -26685,7 +27135,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="123" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B123" s="9">
         <v>0.88490740740740748</v>
       </c>
@@ -26981,7 +27431,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="124" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B124" s="9">
         <v>0.89532407407407411</v>
       </c>
@@ -27277,7 +27727,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="125" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B125" s="9">
         <v>0.90574074074074085</v>
       </c>
@@ -27573,7 +28023,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="126" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B126" s="9">
         <v>0.91615740740740748</v>
       </c>
@@ -27869,7 +28319,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="127" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B127" s="9">
         <v>0.92657407407407411</v>
       </c>
@@ -28165,7 +28615,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="128" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B128" s="9">
         <v>0.93699074074074085</v>
       </c>
@@ -28461,7 +28911,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="129" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B129" s="9">
         <v>0.94740740740740748</v>
       </c>
@@ -28757,7 +29207,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="130" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B130" s="9">
         <v>0.95782407407407411</v>
       </c>
@@ -29053,7 +29503,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="131" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B131" s="9">
         <v>0.96824074074074085</v>
       </c>
@@ -29349,7 +29799,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="132" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B132" s="9">
         <v>0.97865740740740748</v>
       </c>
@@ -29645,7 +30095,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="133" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B133" s="9">
         <v>0.98907407407407411</v>
       </c>
@@ -29941,7 +30391,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="134" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B134" s="9">
         <v>0.99949074074074085</v>
       </c>
@@ -30237,7 +30687,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="135" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B135" s="11">
         <v>1.0099074074074075</v>
       </c>
@@ -30533,7 +30983,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="136" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B136" s="11">
         <v>1.0203240740740742</v>
       </c>
@@ -30829,7 +31279,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="137" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B137" s="11">
         <v>1.0307407407407407</v>
       </c>
@@ -31125,7 +31575,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="138" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B138" s="11">
         <v>1.0411574074074075</v>
       </c>
@@ -31421,7 +31871,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="139" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B139" s="11">
         <v>1.0515740740740742</v>
       </c>
@@ -31717,7 +32167,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="140" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B140" s="11">
         <v>1.0619907407407407</v>
       </c>
@@ -32013,7 +32463,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="141" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B141" s="11">
         <v>1.0724074074074075</v>
       </c>
@@ -32309,7 +32759,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="142" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B142" s="11">
         <v>1.0828240740740742</v>
       </c>
@@ -32605,7 +33055,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="143" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B143" s="11">
         <v>1.0932407407407407</v>
       </c>
@@ -32901,7 +33351,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="144" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B144" s="11">
         <v>1.1036574074074075</v>
       </c>
@@ -33197,7 +33647,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="145" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B145" s="11">
         <v>1.1140740740740742</v>
       </c>
@@ -33493,7 +33943,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="146" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B146" s="11">
         <v>1.1244907407407407</v>
       </c>
@@ -33789,7 +34239,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="147" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B147" s="11">
         <v>1.1349074074074075</v>
       </c>
@@ -34085,7 +34535,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="148" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B148" s="11">
         <v>1.1453240740740742</v>
       </c>
@@ -34381,7 +34831,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="149" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B149" s="11">
         <v>1.1557407407407407</v>
       </c>
@@ -34677,7 +35127,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="150" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B150" s="11">
         <v>1.1661574074074075</v>
       </c>
@@ -34973,7 +35423,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="151" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B151" s="11">
         <v>1.1765740740740742</v>
       </c>
@@ -35269,7 +35719,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="152" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B152" s="11">
         <v>1.1869907407407407</v>
       </c>
@@ -35565,7 +36015,7 @@
         <v>0.70099999999999996</v>
       </c>
     </row>
-    <row r="153" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B153" s="11">
         <v>1.1974074074074075</v>
       </c>
@@ -35861,7 +36311,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="154" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B154" s="11">
         <v>1.2078240740740742</v>
       </c>
@@ -36157,7 +36607,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="155" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B155" s="11">
         <v>1.2182407407407407</v>
       </c>
@@ -36453,7 +36903,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="156" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B156" s="11">
         <v>1.2286574074074075</v>
       </c>
@@ -36749,7 +37199,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="157" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B157" s="11">
         <v>1.2390740740740742</v>
       </c>
@@ -37045,7 +37495,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="158" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B158" s="11">
         <v>1.2494907407407407</v>
       </c>
@@ -37341,7 +37791,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="159" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B159" s="11">
         <v>1.2599074074074075</v>
       </c>
@@ -37637,7 +38087,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="160" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B160" s="11">
         <v>1.2703240740740742</v>
       </c>
@@ -37933,7 +38383,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="161" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B161" s="11">
         <v>1.2807407407407407</v>
       </c>
@@ -38229,7 +38679,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="162" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B162" s="11">
         <v>1.2911574074074075</v>
       </c>
@@ -38525,7 +38975,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="163" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B163" s="11">
         <v>1.3015740740740742</v>
       </c>
@@ -38821,7 +39271,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="164" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B164" s="11">
         <v>1.3119907407407407</v>
       </c>
@@ -39117,7 +39567,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="165" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B165" s="11">
         <v>1.3224074074074075</v>
       </c>
@@ -39413,7 +39863,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="166" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B166" s="11">
         <v>1.3328240740740742</v>
       </c>
@@ -39709,7 +40159,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="167" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B167" s="11">
         <v>1.3432407407407407</v>
       </c>
@@ -40005,7 +40455,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="168" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B168" s="11">
         <v>1.3536574074074075</v>
       </c>
@@ -40301,7 +40751,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="169" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B169" s="11">
         <v>1.3640740740740742</v>
       </c>
@@ -40597,7 +41047,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="170" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B170" s="11">
         <v>1.3744907407407407</v>
       </c>
@@ -40893,7 +41343,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="171" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B171" s="11">
         <v>1.3849074074074075</v>
       </c>
@@ -41189,7 +41639,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="172" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B172" s="11">
         <v>1.3953240740740742</v>
       </c>
@@ -41485,7 +41935,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="173" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B173" s="11">
         <v>1.4057407407407407</v>
       </c>
@@ -41781,7 +42231,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="174" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B174" s="11">
         <v>1.4161574074074075</v>
       </c>
@@ -42077,7 +42527,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="175" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B175" s="11">
         <v>1.4265740740740742</v>
       </c>
@@ -42373,7 +42823,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="176" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B176" s="11">
         <v>1.4369907407407407</v>
       </c>
@@ -42669,7 +43119,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="177" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B177" s="11">
         <v>1.4474074074074075</v>
       </c>
@@ -42965,7 +43415,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="178" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B178" s="11">
         <v>1.4578240740740742</v>
       </c>
@@ -43261,7 +43711,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="179" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B179" s="11">
         <v>1.4682407407407407</v>
       </c>
@@ -43557,7 +44007,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="180" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B180" s="11">
         <v>1.4786574074074075</v>
       </c>
@@ -43853,7 +44303,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="181" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B181" s="11">
         <v>1.4890740740740742</v>
       </c>
@@ -44149,7 +44599,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="182" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B182" s="11">
         <v>1.4994907407407407</v>
       </c>
@@ -44445,7 +44895,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="183" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B183" s="11">
         <v>1.5099074074074075</v>
       </c>
@@ -44741,7 +45191,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="184" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B184" s="11">
         <v>1.5203240740740742</v>
       </c>
@@ -45037,7 +45487,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="185" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B185" s="11">
         <v>1.5307407407407407</v>
       </c>
@@ -45333,7 +45783,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="186" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B186" s="11">
         <v>1.5411574074074075</v>
       </c>
@@ -45629,7 +46079,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="187" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B187" s="11">
         <v>1.5515740740740742</v>
       </c>
@@ -45925,7 +46375,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="188" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B188" s="11">
         <v>1.5619907407407407</v>
       </c>
@@ -46221,7 +46671,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="189" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B189" s="11">
         <v>1.5724074074074075</v>
       </c>
@@ -46517,7 +46967,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="190" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B190" s="11">
         <v>1.5828240740740742</v>
       </c>
@@ -46813,7 +47263,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="191" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B191" s="11">
         <v>1.5932407407407407</v>
       </c>
@@ -47109,7 +47559,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="192" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B192" s="11">
         <v>1.6036574074074075</v>
       </c>
@@ -47405,7 +47855,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="193" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B193" s="11">
         <v>1.6140740740740742</v>
       </c>
@@ -47701,7 +48151,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="194" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B194" s="11">
         <v>1.6244907407407407</v>
       </c>
@@ -47997,7 +48447,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="195" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B195" s="11">
         <v>1.6349074074074075</v>
       </c>
@@ -48293,7 +48743,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="196" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B196" s="11">
         <v>1.6453240740740742</v>
       </c>
@@ -48589,7 +49039,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="197" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B197" s="11">
         <v>1.6557407407407407</v>
       </c>
@@ -48885,7 +49335,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="198" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B198" s="11">
         <v>1.6661574074074075</v>
       </c>
@@ -49181,7 +49631,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="199" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B199" s="11">
         <v>1.6765740740740742</v>
       </c>
@@ -49477,7 +49927,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="200" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B200" s="11">
         <v>1.6869907407407407</v>
       </c>
@@ -49773,7 +50223,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="201" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B201" s="11">
         <v>1.6974074074074075</v>
       </c>
@@ -50069,7 +50519,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="202" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B202" s="11">
         <v>1.7078240740740742</v>
       </c>
@@ -50365,7 +50815,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="203" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B203" s="11">
         <v>1.7182407407407407</v>
       </c>
@@ -50661,7 +51111,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="204" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B204" s="11">
         <v>1.7286574074074075</v>
       </c>
@@ -50957,7 +51407,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="205" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B205" s="11">
         <v>1.7390740740740742</v>
       </c>
@@ -51253,7 +51703,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="206" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B206" s="11">
         <v>1.7494907407407407</v>
       </c>
@@ -51549,7 +51999,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="207" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B207" s="11">
         <v>1.7599074074074075</v>
       </c>
@@ -51845,7 +52295,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="208" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B208" s="11">
         <v>1.7703240740740742</v>
       </c>
@@ -52141,7 +52591,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="209" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B209" s="11">
         <v>1.7807407407407407</v>
       </c>
@@ -52437,7 +52887,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="210" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B210" s="11">
         <v>1.7911574074074075</v>
       </c>
@@ -52733,7 +53183,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="211" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B211" s="11">
         <v>1.8015740740740742</v>
       </c>
@@ -53029,7 +53479,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="212" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B212" s="11">
         <v>1.8119907407407407</v>
       </c>
@@ -53325,7 +53775,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="213" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B213" s="11">
         <v>1.8224074074074075</v>
       </c>
@@ -53621,7 +54071,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="214" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B214" s="11">
         <v>1.8328240740740742</v>
       </c>
@@ -53917,7 +54367,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="215" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B215" s="11">
         <v>1.8432407407407407</v>
       </c>
@@ -54213,7 +54663,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="216" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B216" s="11">
         <v>1.8536574074074075</v>
       </c>
@@ -54509,7 +54959,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="217" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B217" s="11">
         <v>1.8640740740740742</v>
       </c>
@@ -54805,7 +55255,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="218" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B218" s="11">
         <v>1.8744907407407407</v>
       </c>
@@ -55101,7 +55551,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="219" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B219" s="11">
         <v>1.8849074074074075</v>
       </c>
@@ -55397,7 +55847,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="220" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B220" s="11">
         <v>1.8953240740740742</v>
       </c>
@@ -55693,7 +56143,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="221" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B221" s="11">
         <v>1.9057407407407407</v>
       </c>
@@ -55989,7 +56439,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="222" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B222" s="11">
         <v>1.9161574074074075</v>
       </c>
@@ -56285,7 +56735,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="223" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B223" s="11">
         <v>1.9265740740740742</v>
       </c>
@@ -56581,7 +57031,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="224" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B224" s="11">
         <v>1.9369907407407407</v>
       </c>
@@ -56877,7 +57327,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="225" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B225" s="11">
         <v>1.9474074074074075</v>
       </c>
@@ -57173,7 +57623,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="226" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B226" s="11">
         <v>1.9578240740740742</v>
       </c>
@@ -57469,7 +57919,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="227" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B227" s="11">
         <v>1.9682407407407407</v>
       </c>
@@ -57765,7 +58215,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="228" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B228" s="11">
         <v>1.9786574074074075</v>
       </c>
@@ -58061,7 +58511,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="229" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B229" s="11">
         <v>1.9890740740740742</v>
       </c>
@@ -58357,7 +58807,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="230" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B230" s="11">
         <v>1.9994907407407407</v>
       </c>
@@ -58653,7 +59103,7 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="231" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B231" s="11">
         <v>2.0099074074074075</v>
       </c>
@@ -58949,13 +59399,13 @@
         <v>0.69799999999999995</v>
       </c>
     </row>
-    <row r="233" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:99" ht="13" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B233" s="4"/>
     </row>
-    <row r="235" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B235" s="5"/>
       <c r="C235" s="6">
         <v>1</v>
@@ -58994,7 +59444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="236" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B236" s="19" t="s">
         <v>30</v>
       </c>
@@ -59038,7 +59488,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="237" spans="1:99" ht="18" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:99" ht="18" x14ac:dyDescent="0.25">
       <c r="B237" s="20"/>
       <c r="C237" s="13">
         <v>0.91800000000000004</v>
@@ -59080,7 +59530,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="238" spans="1:99" ht="18" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:99" ht="18" x14ac:dyDescent="0.25">
       <c r="B238" s="20"/>
       <c r="C238" s="14">
         <v>3.0740740740740739E-2</v>
@@ -59122,7 +59572,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="239" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B239" s="21"/>
       <c r="C239" s="16" t="s">
         <v>161</v>
@@ -59164,7 +59614,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="240" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B240" s="19" t="s">
         <v>33</v>
       </c>
@@ -59208,7 +59658,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="241" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B241" s="20"/>
       <c r="C241" s="13">
         <v>0.86599999999999999</v>
@@ -59250,7 +59700,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="242" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B242" s="20"/>
       <c r="C242" s="14">
         <v>3.0740740740740739E-2</v>
@@ -59292,7 +59742,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="243" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B243" s="21"/>
       <c r="C243" s="16" t="s">
         <v>161</v>
@@ -59334,7 +59784,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="244" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B244" s="19" t="s">
         <v>44</v>
       </c>
@@ -59378,7 +59828,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="245" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B245" s="20"/>
       <c r="C245" s="13">
         <v>0.98299999999999998</v>
@@ -59420,7 +59870,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="246" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B246" s="20"/>
       <c r="C246" s="14">
         <v>3.0740740740740739E-2</v>
@@ -59462,7 +59912,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="247" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B247" s="21"/>
       <c r="C247" s="16" t="s">
         <v>161</v>
@@ -59504,7 +59954,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="248" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B248" s="19" t="s">
         <v>45</v>
       </c>
@@ -59548,7 +59998,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="249" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B249" s="20"/>
       <c r="C249" s="13">
         <v>0.99299999999999999</v>
@@ -59590,7 +60040,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="250" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B250" s="20"/>
       <c r="C250" s="14">
         <v>0.14532407407407408</v>
@@ -59632,7 +60082,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="251" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B251" s="21"/>
       <c r="C251" s="17">
         <v>5.3414351851851859E-2</v>
@@ -59674,7 +60124,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="252" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B252" s="19" t="s">
         <v>46</v>
       </c>
@@ -59718,7 +60168,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="253" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B253" s="20"/>
       <c r="C253" s="13">
         <v>0.999</v>
@@ -59760,7 +60210,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="254" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B254" s="20"/>
       <c r="C254" s="15">
         <v>1.9786574074074075</v>
@@ -59802,7 +60252,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="255" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B255" s="21"/>
       <c r="C255" s="16" t="s">
         <v>161</v>
@@ -59844,7 +60294,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="256" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B256" s="19" t="s">
         <v>57</v>
       </c>
@@ -59888,7 +60338,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="257" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B257" s="20"/>
       <c r="C257" s="13">
         <v>0.998</v>
@@ -59930,7 +60380,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="258" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B258" s="20"/>
       <c r="C258" s="15">
         <v>1.9161574074074075</v>
@@ -59972,7 +60422,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="259" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B259" s="21"/>
       <c r="C259" s="18">
         <v>1.8826620370370371</v>
@@ -60014,7 +60464,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="260" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B260" s="19" t="s">
         <v>58</v>
       </c>
@@ -60058,7 +60508,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="261" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B261" s="20"/>
       <c r="C261" s="13">
         <v>0.99099999999999999</v>
@@ -60100,7 +60550,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="262" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B262" s="20"/>
       <c r="C262" s="15">
         <v>1.9161574074074075</v>
@@ -60142,7 +60592,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="263" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B263" s="21"/>
       <c r="C263" s="18">
         <v>1.9398958333333332</v>
@@ -60184,7 +60634,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="264" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B264" s="19" t="s">
         <v>59</v>
       </c>
@@ -60228,7 +60678,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="265" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B265" s="20"/>
       <c r="C265" s="13">
         <v>0.97399999999999998</v>
@@ -60270,7 +60720,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="266" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B266" s="20"/>
       <c r="C266" s="14">
         <v>3.0740740740740739E-2</v>
@@ -60312,7 +60762,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="267" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B267" s="21"/>
       <c r="C267" s="16" t="s">
         <v>161</v>
@@ -60370,4 +60820,1579 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500D04F3-DDE4-44FE-9527-F9FD9D2DBAEC}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2237EE-4CF6-41A1-854F-8BE30896F440}">
+  <dimension ref="A1:D97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="B84:D84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="C66" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="C78" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D78" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="D80" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D81" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B84" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="C84" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D84" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="C86" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D86" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="C87" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D87" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B88" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="C88" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D88" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B89" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C89" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D89" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B90" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C90" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D90" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B91" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="C91" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D91" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B92" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D92" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B93" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="C93" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D93" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B94" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C94" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D94" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B95" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="C95" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B96" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="C96" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D96" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B97" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C97" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D97" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>